<commit_message>
Se elimina formularios que ya no se requieren
</commit_message>
<xml_diff>
--- a/SistemaInformacionCun2/Modelo bd .xlsb.xlsx
+++ b/SistemaInformacionCun2/Modelo bd .xlsb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Source\Repos\SistemasInformacionCun\SistemaInformacionCun2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhurtado\Desktop\Documentos\Visual\SistemaInformacionCun2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1429BB-A270-47CE-B55E-6B47312FAD61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB009528-683C-4F41-BD09-1265C9FB3748}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="7470" windowHeight="2595" activeTab="4" xr2:uid="{F70D0863-ADA0-4BEF-8552-167FE4C13056}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="Disco duro" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -747,7 +746,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>